<commit_message>
working check-in princ calc upload
</commit_message>
<xml_diff>
--- a/aws_calc/EC2_Template.xlsx
+++ b/aws_calc/EC2_Template.xlsx
@@ -867,7 +867,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1543,126 +1543,6 @@
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r7g.2xlarge', 'vCPU': '8', 'Memory': '64', 'PricePerUnit': '0.5583'}</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>r7g.2xlarge</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>0.5583</t>
-        </is>
-      </c>
-      <c r="L39" t="n">
-        <v>407.559</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r6i.4xlarge', 'vCPU': '16', 'Memory': '96 GiB', 'PricePerUnit': '1.008'}</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>r6i.4xlarge</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>1.008</t>
-        </is>
-      </c>
-      <c r="L40" t="n">
-        <v>735.84</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1674,7 +1554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:R1029"/>
+  <dimension ref="A2:R1003"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1819,18 +1699,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13">
-        <f>IF(ISBLANK(H4),0,1)</f>
-        <v/>
+      <c r="A4" s="13" t="inlineStr">
+        <is>
+          <t>AA00001527</t>
+        </is>
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>Production</t>
+          <t>AA00001527</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
         <is>
-          <t>Test1</t>
+          <t>ASX1 - DEV - OZ - MSSQL</t>
         </is>
       </c>
       <c r="D4" s="25" t="inlineStr">
@@ -1840,12 +1721,12 @@
       </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
-          <t>Linux</t>
+          <t>Windows Server</t>
         </is>
       </c>
       <c r="F4" s="23" t="inlineStr">
         <is>
-          <t>t4g.nano</t>
+          <t>r5a.2xlarge</t>
         </is>
       </c>
       <c r="G4" s="19" t="inlineStr">
@@ -1853,10 +1734,12 @@
           <t>Shared Instances</t>
         </is>
       </c>
-      <c r="H4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="n"/>
+      <c r="H4" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" s="6" t="inlineStr"/>
       <c r="J4" s="15" t="inlineStr">
         <is>
           <t>Always On</t>
@@ -1864,7 +1747,7 @@
       </c>
       <c r="K4" s="13" t="inlineStr">
         <is>
-          <t>3 Yr All Upfront Compute Savings Plan</t>
+          <t>On-Demand</t>
         </is>
       </c>
       <c r="L4" s="13" t="inlineStr">
@@ -1872,42 +1755,51 @@
           <t>General Purpose SSD (gp3)</t>
         </is>
       </c>
-      <c r="M4" s="6" t="n">
-        <v>55</v>
-      </c>
-      <c r="N4" s="6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="O4" s="6" t="n">
-        <v>500</v>
+      <c r="M4" s="6" t="inlineStr">
+        <is>
+          <t>3500</t>
+        </is>
+      </c>
+      <c r="N4" s="6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O4" s="6" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
       <c r="P4" s="6" t="inlineStr">
         <is>
-          <t>Hourly</t>
-        </is>
-      </c>
-      <c r="Q4" s="6" t="n">
-        <v>3000</v>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="Q4" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13">
-        <f>IF(ISBLANK(H5),0,1)</f>
-        <v/>
+      <c r="A5" s="13" t="inlineStr">
+        <is>
+          <t>AA00003081</t>
+        </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>Beta</t>
+          <t>AA00003081</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
         <is>
-          <t>Test2</t>
+          <t>ASX1 - PRD - CPZ - MSSQL</t>
         </is>
       </c>
       <c r="D5" s="22" t="inlineStr">
         <is>
-          <t>us-east-2</t>
+          <t>us-east-1</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr">
@@ -1917,7 +1809,7 @@
       </c>
       <c r="F5" s="24" t="inlineStr">
         <is>
-          <t>c5.4xlarge</t>
+          <t>r7i.4xlarge</t>
         </is>
       </c>
       <c r="G5" s="5" t="inlineStr">
@@ -1925,15 +1817,15 @@
           <t>Shared Instances</t>
         </is>
       </c>
-      <c r="H5" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>167</v>
-      </c>
+      <c r="H5" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" s="6" t="inlineStr"/>
       <c r="J5" s="14" t="inlineStr">
         <is>
-          <t>Hours/Week</t>
+          <t>Always On</t>
         </is>
       </c>
       <c r="K5" s="5" t="inlineStr">
@@ -1943,61 +1835,200 @@
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>General Purpose SSD (gp2)</t>
-        </is>
-      </c>
-      <c r="M5" s="6" t="n">
-        <v>2924</v>
-      </c>
-      <c r="N5" s="6" t="n"/>
-      <c r="O5" s="6" t="n"/>
+          <t>General Purpose SSD (gp3)</t>
+        </is>
+      </c>
+      <c r="M5" s="6" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="N5" s="6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O5" s="6" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
       <c r="P5" s="6" t="inlineStr">
         <is>
-          <t>No snapshot storage</t>
-        </is>
-      </c>
-      <c r="Q5" s="6" t="n"/>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="Q5" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="n"/>
-      <c r="B6" s="13" t="n"/>
-      <c r="C6" s="13" t="n"/>
-      <c r="D6" s="22" t="n"/>
-      <c r="E6" s="5" t="n"/>
-      <c r="F6" s="24" t="n"/>
-      <c r="G6" s="5" t="n"/>
-      <c r="H6" s="6" t="n"/>
-      <c r="I6" s="6" t="n"/>
-      <c r="J6" s="14" t="n"/>
-      <c r="K6" s="5" t="n"/>
-      <c r="L6" s="5" t="n"/>
-      <c r="M6" s="6" t="n"/>
-      <c r="N6" s="6" t="n"/>
-      <c r="O6" s="6" t="n"/>
-      <c r="P6" s="6" t="n"/>
-      <c r="Q6" s="6" t="n"/>
+      <c r="A6" s="13" t="inlineStr">
+        <is>
+          <t>AA00002512</t>
+        </is>
+      </c>
+      <c r="B6" s="13" t="inlineStr">
+        <is>
+          <t>AA00002512</t>
+        </is>
+      </c>
+      <c r="C6" s="13" t="inlineStr">
+        <is>
+          <t>SJX1 - ATN - SNP - MSSQL</t>
+        </is>
+      </c>
+      <c r="D6" s="22" t="inlineStr">
+        <is>
+          <t>us-east-1</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>Windows Server</t>
+        </is>
+      </c>
+      <c r="F6" s="24" t="inlineStr">
+        <is>
+          <t>r6a.2xlarge</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Shared Instances</t>
+        </is>
+      </c>
+      <c r="H6" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I6" s="6" t="inlineStr"/>
+      <c r="J6" s="14" t="inlineStr">
+        <is>
+          <t>Always On</t>
+        </is>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>On-Demand</t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="inlineStr">
+        <is>
+          <t>General Purpose SSD (gp3)</t>
+        </is>
+      </c>
+      <c r="M6" s="6" t="inlineStr">
+        <is>
+          <t>3610</t>
+        </is>
+      </c>
+      <c r="N6" s="6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O6" s="6" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="P6" s="6" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="Q6" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="13">
-        <f>IF(ISBLANK(H7),0,1)</f>
-        <v/>
-      </c>
-      <c r="B7" s="13" t="n"/>
-      <c r="C7" s="13" t="n"/>
-      <c r="D7" s="22" t="n"/>
-      <c r="E7" s="5" t="n"/>
-      <c r="F7" s="24" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="6" t="n"/>
-      <c r="I7" s="6" t="n"/>
-      <c r="J7" s="14" t="n"/>
-      <c r="K7" s="5" t="n"/>
-      <c r="L7" s="5" t="n"/>
-      <c r="M7" s="6" t="n"/>
-      <c r="N7" s="6" t="n"/>
-      <c r="O7" s="6" t="n"/>
-      <c r="P7" s="6" t="n"/>
-      <c r="Q7" s="6" t="n"/>
+      <c r="A7" s="13" t="inlineStr">
+        <is>
+          <t>AA00004362</t>
+        </is>
+      </c>
+      <c r="B7" s="13" t="inlineStr">
+        <is>
+          <t>AA00004362</t>
+        </is>
+      </c>
+      <c r="C7" s="13" t="inlineStr">
+        <is>
+          <t>SJX1 - ATN - SNP - MSSQL</t>
+        </is>
+      </c>
+      <c r="D7" s="22" t="inlineStr">
+        <is>
+          <t>us-east-1</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>Windows Server</t>
+        </is>
+      </c>
+      <c r="F7" s="24" t="inlineStr">
+        <is>
+          <t>r5a.4xlarge</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>Shared Instances</t>
+        </is>
+      </c>
+      <c r="H7" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I7" s="6" t="inlineStr"/>
+      <c r="J7" s="14" t="inlineStr">
+        <is>
+          <t>Always On</t>
+        </is>
+      </c>
+      <c r="K7" s="5" t="inlineStr">
+        <is>
+          <t>On-Demand</t>
+        </is>
+      </c>
+      <c r="L7" s="5" t="inlineStr">
+        <is>
+          <t>General Purpose SSD (gp3)</t>
+        </is>
+      </c>
+      <c r="M7" s="6" t="inlineStr">
+        <is>
+          <t>5610</t>
+        </is>
+      </c>
+      <c r="N7" s="6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="O7" s="6" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="P7" s="6" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="Q7" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="13">
@@ -23910,1574 +23941,6 @@
       <c r="O1003" s="13" t="n"/>
       <c r="P1003" s="29" t="n"/>
       <c r="Q1003" s="13" t="n"/>
-    </row>
-    <row r="1004">
-      <c r="A1004" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1004" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1004" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1004" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1004" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1004" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1004" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1004" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1004" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r7a.large', 'vCPU': '8', 'Memory': '49.3 GiB', 'PricePerUnit': '0.62'}</t>
-        </is>
-      </c>
-      <c r="J1004" t="inlineStr">
-        <is>
-          <t>r7a.large</t>
-        </is>
-      </c>
-      <c r="K1004" t="inlineStr">
-        <is>
-          <t>0.62</t>
-        </is>
-      </c>
-      <c r="L1004" t="n">
-        <v>452.6</v>
-      </c>
-    </row>
-    <row r="1005">
-      <c r="A1005" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1005" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1005" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1005" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1005" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1005" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1005" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1005" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1005" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r6i.12xlarge', 'vCPU': '48', 'Memory': '384 GiB', 'PricePerUnit': '3.5424'}</t>
-        </is>
-      </c>
-      <c r="J1005" t="inlineStr">
-        <is>
-          <t>r6i.12xlarge</t>
-        </is>
-      </c>
-      <c r="K1005" t="inlineStr">
-        <is>
-          <t>3.5424</t>
-        </is>
-      </c>
-      <c r="L1005" t="n">
-        <v>2585.952</v>
-      </c>
-    </row>
-    <row r="1006">
-      <c r="A1006" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1006" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1006" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1006" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1006" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1006" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1006" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1006" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1006" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J1006" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="K1006" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L1006" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="1007">
-      <c r="A1007" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1007" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1007" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1007" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1007" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1007" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1007" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1007" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1007" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r6i.12xlarge', 'vCPU': '48', 'Memory': '384 GiB', 'PricePerUnit': '3.5424'}</t>
-        </is>
-      </c>
-      <c r="J1007" t="inlineStr">
-        <is>
-          <t>r6i.12xlarge</t>
-        </is>
-      </c>
-      <c r="K1007" t="inlineStr">
-        <is>
-          <t>3.5424</t>
-        </is>
-      </c>
-      <c r="L1007" t="n">
-        <v>2585.952</v>
-      </c>
-    </row>
-    <row r="1008">
-      <c r="A1008" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1008" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1008" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1008" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1008" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1008" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1008" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1008" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1008" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'u7i-16tb.224xlarge', 'vCPU': '896', 'Memory': '16384 GiB', 'PricePerUnit': '203.84'}</t>
-        </is>
-      </c>
-      <c r="J1008" t="inlineStr">
-        <is>
-          <t>u7i-16tb.224xlarge</t>
-        </is>
-      </c>
-      <c r="K1008" t="inlineStr">
-        <is>
-          <t>203.84</t>
-        </is>
-      </c>
-      <c r="L1008" t="n">
-        <v>148803.2</v>
-      </c>
-    </row>
-    <row r="1009">
-      <c r="A1009" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1009" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1009" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1009" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1009" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1009" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1009" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1009" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1009" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'u7in-16tb.192xlarge', 'vCPU': '16', 'Memory': '96 GiB', 'PricePerUnit': '305.885'}</t>
-        </is>
-      </c>
-      <c r="J1009" t="inlineStr">
-        <is>
-          <t>u7in-16tb.192xlarge</t>
-        </is>
-      </c>
-      <c r="K1009" t="inlineStr">
-        <is>
-          <t>305.885</t>
-        </is>
-      </c>
-      <c r="L1009" t="n">
-        <v>223296.05</v>
-      </c>
-    </row>
-    <row r="1010">
-      <c r="A1010" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1010" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1010" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1010" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1010" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1010" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1010" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1010" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1010" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5d.2xlarge', 'vCPU': '8', 'Memory': '61 GiB', 'PricePerUnit': '0.576'}</t>
-        </is>
-      </c>
-      <c r="J1010" t="inlineStr">
-        <is>
-          <t>r5d.2xlarge</t>
-        </is>
-      </c>
-      <c r="K1010" t="inlineStr">
-        <is>
-          <t>0.576</t>
-        </is>
-      </c>
-      <c r="L1010" t="n">
-        <v>420.48</v>
-      </c>
-    </row>
-    <row r="1011">
-      <c r="A1011" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1011" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1011" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1011" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1011" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1011" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1011" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1011" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1011" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r6g.4xlarge', 'vCPU': '16', 'Memory': '128 GiB', 'PricePerUnit': '0.8064'}</t>
-        </is>
-      </c>
-      <c r="J1011" t="inlineStr">
-        <is>
-          <t>r6g.4xlarge</t>
-        </is>
-      </c>
-      <c r="K1011" t="inlineStr">
-        <is>
-          <t>0.8064</t>
-        </is>
-      </c>
-      <c r="L1011" t="n">
-        <v>588.672</v>
-      </c>
-    </row>
-    <row r="1012">
-      <c r="A1012" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1012" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1012" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1012" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1012" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1012" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1012" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1012" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1012" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5a.2xlarge', 'vCPU': '8', 'Memory': '61', 'PricePerUnit': '0.466'}</t>
-        </is>
-      </c>
-      <c r="J1012" t="inlineStr">
-        <is>
-          <t>r5a.2xlarge</t>
-        </is>
-      </c>
-      <c r="K1012" t="inlineStr">
-        <is>
-          <t>0.466</t>
-        </is>
-      </c>
-      <c r="L1012" t="n">
-        <v>340.18</v>
-      </c>
-    </row>
-    <row r="1013">
-      <c r="A1013" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1013" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1013" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1013" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1013" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1013" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1013" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1013" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1013" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J1013" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="K1013" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L1013" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="1014">
-      <c r="A1014" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1014" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1014" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1014" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1014" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1014" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1014" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1014" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1014" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5d.2xlarge', 'vCPU': '8', 'Memory': '61 GiB', 'PricePerUnit': '0.576'}</t>
-        </is>
-      </c>
-      <c r="J1014" t="inlineStr">
-        <is>
-          <t>r5d.2xlarge</t>
-        </is>
-      </c>
-      <c r="K1014" t="inlineStr">
-        <is>
-          <t>0.576</t>
-        </is>
-      </c>
-      <c r="L1014" t="n">
-        <v>420.48</v>
-      </c>
-    </row>
-    <row r="1015">
-      <c r="A1015" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1015" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1015" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1015" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1015" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1015" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1015" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1015" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1015" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5.large', 'vCPU': '2', 'Memory': '15.75 GiB', 'PricePerUnit': '0.0683'}</t>
-        </is>
-      </c>
-      <c r="J1015" t="inlineStr">
-        <is>
-          <t>r5.large</t>
-        </is>
-      </c>
-      <c r="K1015" t="inlineStr">
-        <is>
-          <t>0.0683</t>
-        </is>
-      </c>
-      <c r="L1015" t="n">
-        <v>49.859</v>
-      </c>
-    </row>
-    <row r="1016">
-      <c r="A1016" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1016" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1016" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1016" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1016" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1016" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1016" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1016" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1016" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5d.large', 'vCPU': '2', 'Memory': '38.4', 'PricePerUnit': '0.129'}</t>
-        </is>
-      </c>
-      <c r="J1016" t="inlineStr">
-        <is>
-          <t>r5d.large</t>
-        </is>
-      </c>
-      <c r="K1016" t="inlineStr">
-        <is>
-          <t>0.129</t>
-        </is>
-      </c>
-      <c r="L1016" t="n">
-        <v>94.17</v>
-      </c>
-    </row>
-    <row r="1017">
-      <c r="A1017" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1017" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1017" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1017" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1017" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1017" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1017" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1017" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1017" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5n.large', 'vCPU': '16', 'Memory': '97 GiB', 'PricePerUnit': '0.023'}</t>
-        </is>
-      </c>
-      <c r="J1017" t="inlineStr">
-        <is>
-          <t>r5n.large</t>
-        </is>
-      </c>
-      <c r="K1017" t="inlineStr">
-        <is>
-          <t>0.023</t>
-        </is>
-      </c>
-      <c r="L1017" t="n">
-        <v>16.79</v>
-      </c>
-    </row>
-    <row r="1018">
-      <c r="A1018" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1018" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1018" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1018" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1018" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1018" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1018" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1018" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1018" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5d.2xlarge', 'vCPU': '8', 'Memory': '61 GiB', 'PricePerUnit': '0.576'}</t>
-        </is>
-      </c>
-      <c r="J1018" t="inlineStr">
-        <is>
-          <t>r5d.2xlarge</t>
-        </is>
-      </c>
-      <c r="K1018" t="inlineStr">
-        <is>
-          <t>0.576</t>
-        </is>
-      </c>
-      <c r="L1018" t="n">
-        <v>420.48</v>
-      </c>
-    </row>
-    <row r="1019">
-      <c r="A1019" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1019" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1019" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1019" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1019" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1019" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1019" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1019" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1019" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5n.xlarge', 'vCPU': '16', 'Memory': '96 GiB', 'PricePerUnit': '1.22'}</t>
-        </is>
-      </c>
-      <c r="J1019" t="inlineStr">
-        <is>
-          <t>r5n.xlarge</t>
-        </is>
-      </c>
-      <c r="K1019" t="inlineStr">
-        <is>
-          <t>1.22</t>
-        </is>
-      </c>
-      <c r="L1019" t="n">
-        <v>890.6</v>
-      </c>
-    </row>
-    <row r="1020">
-      <c r="A1020" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1020" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1020" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1020" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1020" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1020" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1020" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1020" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1020" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5d.large', 'vCPU': '1', 'Memory': '48', 'PricePerUnit': '0.078'}</t>
-        </is>
-      </c>
-      <c r="J1020" t="inlineStr">
-        <is>
-          <t>r5d.large</t>
-        </is>
-      </c>
-      <c r="K1020" t="inlineStr">
-        <is>
-          <t>0.078</t>
-        </is>
-      </c>
-      <c r="L1020" t="n">
-        <v>56.94</v>
-      </c>
-    </row>
-    <row r="1021">
-      <c r="A1021" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1021" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1021" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1021" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1021" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1021" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1021" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1021" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1021" t="inlineStr">
-        <is>
-          <t>{"Instance Type": "r5.xlarge", "vCPU": "2", "Memory": "32 GiB", "PricePerUnit": "0.144"}</t>
-        </is>
-      </c>
-      <c r="J1021" t="inlineStr">
-        <is>
-          <t>r5.xlarge</t>
-        </is>
-      </c>
-      <c r="K1021" t="inlineStr">
-        <is>
-          <t>0.144</t>
-        </is>
-      </c>
-      <c r="L1021" t="n">
-        <v>105.12</v>
-      </c>
-    </row>
-    <row r="1022">
-      <c r="A1022" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1022" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1022" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1022" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1022" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1022" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1022" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1022" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1022" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5a.2xlarge', 'vCPU': '8', 'Memory': '61 GiB', 'PricePerUnit': '0.466'}</t>
-        </is>
-      </c>
-      <c r="J1022" t="inlineStr">
-        <is>
-          <t>r5a.2xlarge</t>
-        </is>
-      </c>
-      <c r="K1022" t="inlineStr">
-        <is>
-          <t>0.466</t>
-        </is>
-      </c>
-      <c r="L1022" t="n">
-        <v>340.18</v>
-      </c>
-    </row>
-    <row r="1023">
-      <c r="A1023" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1023" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1023" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1023" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1023" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1023" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1023" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1023" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1023" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5n.xlarge', 'vCPU': '16', 'Memory': '96 GiB', 'PricePerUnit': '1.22'}</t>
-        </is>
-      </c>
-      <c r="J1023" t="inlineStr">
-        <is>
-          <t>r5n.xlarge</t>
-        </is>
-      </c>
-      <c r="K1023" t="inlineStr">
-        <is>
-          <t>1.22</t>
-        </is>
-      </c>
-      <c r="L1023" t="n">
-        <v>890.6</v>
-      </c>
-    </row>
-    <row r="1024">
-      <c r="A1024" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1024" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1024" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1024" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1024" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1024" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1024" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1024" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1024" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5d.2xlarge', 'vCPU': '8', 'Memory': '61 GiB', 'PricePerUnit': '0.576'}</t>
-        </is>
-      </c>
-      <c r="J1024" t="inlineStr">
-        <is>
-          <t>r5d.2xlarge</t>
-        </is>
-      </c>
-      <c r="K1024" t="inlineStr">
-        <is>
-          <t>0.576</t>
-        </is>
-      </c>
-      <c r="L1024" t="n">
-        <v>420.48</v>
-      </c>
-    </row>
-    <row r="1025">
-      <c r="A1025" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1025" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1025" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1025" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1025" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1025" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1025" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1025" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1025" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5n.xlarge', 'vCPU': '4', 'Memory': '60', 'PricePerUnit': '0.08336'}</t>
-        </is>
-      </c>
-      <c r="J1025" t="inlineStr">
-        <is>
-          <t>r5n.xlarge</t>
-        </is>
-      </c>
-      <c r="K1025" t="inlineStr">
-        <is>
-          <t>0.08336</t>
-        </is>
-      </c>
-      <c r="L1025" t="n">
-        <v>60.8528</v>
-      </c>
-    </row>
-    <row r="1026">
-      <c r="A1026" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1026" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1026" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1026" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1026" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1026" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1026" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1026" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1026" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5a.2xlarge', 'vCPU': '8', 'Memory': '61 GiB', 'PricePerUnit': '0.466'}</t>
-        </is>
-      </c>
-      <c r="J1026" t="inlineStr">
-        <is>
-          <t>r5a.2xlarge</t>
-        </is>
-      </c>
-      <c r="K1026" t="inlineStr">
-        <is>
-          <t>0.466</t>
-        </is>
-      </c>
-      <c r="L1026" t="n">
-        <v>340.18</v>
-      </c>
-    </row>
-    <row r="1027">
-      <c r="A1027" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1027" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1027" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1027" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1027" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1027" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1027" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1027" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1027" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J1027" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="K1027" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L1027" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="1028">
-      <c r="A1028" t="inlineStr">
-        <is>
-          <t>AA00001527</t>
-        </is>
-      </c>
-      <c r="B1028" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1028" t="inlineStr">
-        <is>
-          <t>DEV</t>
-        </is>
-      </c>
-      <c r="D1028" t="inlineStr">
-        <is>
-          <t>OZ</t>
-        </is>
-      </c>
-      <c r="E1028" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F1028" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="G1028" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1028" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="I1028" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J1028" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="K1028" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L1028" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="1029">
-      <c r="A1029" t="inlineStr">
-        <is>
-          <t>AA00003081</t>
-        </is>
-      </c>
-      <c r="B1029" t="inlineStr">
-        <is>
-          <t>ASX1</t>
-        </is>
-      </c>
-      <c r="C1029" t="inlineStr">
-        <is>
-          <t>PRD</t>
-        </is>
-      </c>
-      <c r="D1029" t="inlineStr">
-        <is>
-          <t>CPZ</t>
-        </is>
-      </c>
-      <c r="E1029" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="F1029" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="G1029" t="inlineStr">
-        <is>
-          <t>MSSQL</t>
-        </is>
-      </c>
-      <c r="H1029" t="inlineStr">
-        <is>
-          <t>9000</t>
-        </is>
-      </c>
-      <c r="I1029" t="inlineStr">
-        <is>
-          <t>{'Instance Type': 'r5n.large', 'vCPU': '1', 'Memory': '8 GiB', 'PricePerUnit': '0.34'}</t>
-        </is>
-      </c>
-      <c r="J1029" t="inlineStr">
-        <is>
-          <t>r5n.large</t>
-        </is>
-      </c>
-      <c r="K1029" t="inlineStr">
-        <is>
-          <t>0.34</t>
-        </is>
-      </c>
-      <c r="L1029" t="n">
-        <v>248.2</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>